<commit_message>
partial success in relevant data to print
</commit_message>
<xml_diff>
--- a/data/Grapes-Vineyard A.xlsx
+++ b/data/Grapes-Vineyard A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matan.lindenbaum/PycharmProjects/pythonProject/pythonProject2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6142FCA-F478-A54F-B367-19741F56A197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C546CA8-2315-8441-AA2D-244A441B586C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="500" windowWidth="38380" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,10 +558,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -63396,18 +63396,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63582,14 +63582,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A414202-2958-43FC-B63F-EAD4CF9E4B91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BEC98ED-18A5-49F4-B989-A89EFA2B07F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -63602,6 +63594,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A414202-2958-43FC-B63F-EAD4CF9E4B91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
1. adding correlation matrix by vinyards. 2. adding matrix print with same y axis
</commit_message>
<xml_diff>
--- a/data/Grapes-Vineyard A.xlsx
+++ b/data/Grapes-Vineyard A.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matan.lindenbaum/PycharmProjects/pythonProject/pythonProject2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C546CA8-2315-8441-AA2D-244A441B586C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45F8E2-CA23-DA4C-93A8-0FBADBD4BA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AH$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -561,7 +564,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1:AG1"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -63391,26 +63394,12 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AH1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E11EBB08781AF04083B0C426118520C6" ma:contentTypeVersion="5" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="05a6f3e011c48739af6276ee7c779680">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="76caa081-fc44-4d2c-bd81-6f9a75f04feb" xmlns:ns4="0a540cde-0ccb-4e9b-9eab-821ccdced025" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a57451f225ea35e0c8165fb99c7c6a7" ns3:_="" ns4:_="">
     <xsd:import namespace="76caa081-fc44-4d2c-bd81-6f9a75f04feb"/>
@@ -63581,32 +63570,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BEC98ED-18A5-49F4-B989-A89EFA2B07F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="76caa081-fc44-4d2c-bd81-6f9a75f04feb"/>
-    <ds:schemaRef ds:uri="0a540cde-0ccb-4e9b-9eab-821ccdced025"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A414202-2958-43FC-B63F-EAD4CF9E4B91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90A26205-8641-4874-B98E-9B4A8A78A738}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -63623,4 +63602,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A414202-2958-43FC-B63F-EAD4CF9E4B91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BEC98ED-18A5-49F4-B989-A89EFA2B07F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="76caa081-fc44-4d2c-bd81-6f9a75f04feb"/>
+    <ds:schemaRef ds:uri="0a540cde-0ccb-4e9b-9eab-821ccdced025"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>